<commit_message>
fix mass calculator CRITICAL
</commit_message>
<xml_diff>
--- a/data/yannis/output/processed_e.xlsx
+++ b/data/yannis/output/processed_e.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -552,7 +552,7 @@
         <v>5.05</v>
       </c>
       <c r="G2" t="n">
-        <v>1.59</v>
+        <v>1.02</v>
       </c>
       <c r="H2" t="n">
         <v>-73.09</v>
@@ -570,7 +570,7 @@
         <v>3.04</v>
       </c>
       <c r="M2" t="n">
-        <v>0.96</v>
+        <v>0.63</v>
       </c>
       <c r="N2" t="n">
         <v>-23.74</v>
@@ -588,7 +588,7 @@
         <v>5.05</v>
       </c>
       <c r="S2" t="n">
-        <v>1.06</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -613,7 +613,7 @@
         <v>5.05</v>
       </c>
       <c r="G3" t="n">
-        <v>1.59</v>
+        <v>1.02</v>
       </c>
       <c r="H3" t="n">
         <v>-73.09</v>
@@ -631,7 +631,7 @@
         <v>3.04</v>
       </c>
       <c r="M3" t="n">
-        <v>0.96</v>
+        <v>0.63</v>
       </c>
       <c r="N3" t="n">
         <v>-23.74</v>
@@ -649,7 +649,7 @@
         <v>5.05</v>
       </c>
       <c r="S3" t="n">
-        <v>1.06</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4">
@@ -674,7 +674,7 @@
         <v>4.83</v>
       </c>
       <c r="G4" t="n">
-        <v>1.19</v>
+        <v>0.77</v>
       </c>
       <c r="H4" t="n">
         <v>-92.5</v>
@@ -692,7 +692,7 @@
         <v>3.23</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="N4" t="n">
         <v>-30.97</v>
@@ -710,7 +710,7 @@
         <v>4.83</v>
       </c>
       <c r="S4" t="n">
-        <v>0.99</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="5">
@@ -735,7 +735,7 @@
         <v>4.83</v>
       </c>
       <c r="G5" t="n">
-        <v>1.19</v>
+        <v>0.77</v>
       </c>
       <c r="H5" t="n">
         <v>-93.90000000000001</v>
@@ -753,7 +753,7 @@
         <v>3.24</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="N5" t="n">
         <v>-31.02</v>
@@ -771,7 +771,7 @@
         <v>4.83</v>
       </c>
       <c r="S5" t="n">
-        <v>0.99</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="6">
@@ -796,7 +796,7 @@
         <v>4.84</v>
       </c>
       <c r="G6" t="n">
-        <v>1.19</v>
+        <v>0.77</v>
       </c>
       <c r="H6" t="n">
         <v>-93.70999999999999</v>
@@ -814,7 +814,7 @@
         <v>3.24</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="N6" t="n">
         <v>-30.8</v>
@@ -832,7 +832,7 @@
         <v>4.84</v>
       </c>
       <c r="S6" t="n">
-        <v>0.97</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="7">
@@ -857,7 +857,7 @@
         <v>4.84</v>
       </c>
       <c r="G7" t="n">
-        <v>1.07</v>
+        <v>0.66</v>
       </c>
       <c r="H7" t="n">
         <v>-93.26000000000001</v>
@@ -875,7 +875,7 @@
         <v>3.23</v>
       </c>
       <c r="M7" t="n">
-        <v>0.75</v>
+        <v>0.47</v>
       </c>
       <c r="N7" t="n">
         <v>-30.64</v>
@@ -893,7 +893,7 @@
         <v>4.84</v>
       </c>
       <c r="S7" t="n">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="8">
@@ -918,7 +918,7 @@
         <v>4.84</v>
       </c>
       <c r="G8" t="n">
-        <v>1.07</v>
+        <v>0.66</v>
       </c>
       <c r="H8" t="n">
         <v>-93.26000000000001</v>
@@ -936,7 +936,7 @@
         <v>3.23</v>
       </c>
       <c r="M8" t="n">
-        <v>0.75</v>
+        <v>0.47</v>
       </c>
       <c r="N8" t="n">
         <v>-30.64</v>
@@ -954,7 +954,7 @@
         <v>4.84</v>
       </c>
       <c r="S8" t="n">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="9">
@@ -979,7 +979,7 @@
         <v>4.84</v>
       </c>
       <c r="G9" t="n">
-        <v>1.19</v>
+        <v>0.77</v>
       </c>
       <c r="H9" t="n">
         <v>-93.70999999999999</v>
@@ -997,7 +997,7 @@
         <v>3.24</v>
       </c>
       <c r="M9" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="N9" t="n">
         <v>-30.8</v>
@@ -1015,7 +1015,7 @@
         <v>4.84</v>
       </c>
       <c r="S9" t="n">
-        <v>0.97</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="10">
@@ -1040,7 +1040,7 @@
         <v>4.83</v>
       </c>
       <c r="G10" t="n">
-        <v>1.19</v>
+        <v>0.77</v>
       </c>
       <c r="H10" t="n">
         <v>-93.90000000000001</v>
@@ -1058,7 +1058,7 @@
         <v>3.24</v>
       </c>
       <c r="M10" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="N10" t="n">
         <v>-31.02</v>
@@ -1076,7 +1076,7 @@
         <v>4.83</v>
       </c>
       <c r="S10" t="n">
-        <v>0.99</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="11">
@@ -1101,7 +1101,7 @@
         <v>4.83</v>
       </c>
       <c r="G11" t="n">
-        <v>1.19</v>
+        <v>0.77</v>
       </c>
       <c r="H11" t="n">
         <v>-92.5</v>
@@ -1119,7 +1119,7 @@
         <v>3.23</v>
       </c>
       <c r="M11" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="N11" t="n">
         <v>-30.97</v>
@@ -1137,7 +1137,7 @@
         <v>4.83</v>
       </c>
       <c r="S11" t="n">
-        <v>0.99</v>
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried with new precision
</commit_message>
<xml_diff>
--- a/data/yannis/output/processed_e.xlsx
+++ b/data/yannis/output/processed_e.xlsx
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-93.23999999999999</v>
+        <v>-93.23</v>
       </c>
       <c r="C4" t="n">
         <v>17.88</v>
@@ -787,7 +787,7 @@
         <v>17.88</v>
       </c>
       <c r="D6" t="n">
-        <v>30.07</v>
+        <v>30.06</v>
       </c>
       <c r="E6" t="n">
         <v>5.62</v>
@@ -805,7 +805,7 @@
         <v>-17.88</v>
       </c>
       <c r="J6" t="n">
-        <v>30.07</v>
+        <v>30.06</v>
       </c>
       <c r="K6" t="n">
         <v>5.62</v>
@@ -970,7 +970,7 @@
         <v>17.88</v>
       </c>
       <c r="D9" t="n">
-        <v>30.07</v>
+        <v>30.06</v>
       </c>
       <c r="E9" t="n">
         <v>5.62</v>
@@ -988,7 +988,7 @@
         <v>-17.88</v>
       </c>
       <c r="J9" t="n">
-        <v>30.07</v>
+        <v>30.06</v>
       </c>
       <c r="K9" t="n">
         <v>5.62</v>
@@ -1086,7 +1086,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-93.23999999999999</v>
+        <v>-93.23</v>
       </c>
       <c r="C11" t="n">
         <v>17.88</v>

</xml_diff>

<commit_message>
Changed my file again
</commit_message>
<xml_diff>
--- a/data/yannis/output/processed_e.xlsx
+++ b/data/yannis/output/processed_e.xlsx
@@ -543,16 +543,16 @@
         <v>17.88</v>
       </c>
       <c r="D2" t="n">
-        <v>29.71</v>
+        <v>29.705</v>
       </c>
       <c r="E2" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F2" t="n">
-        <v>5.05</v>
+        <v>5.051</v>
       </c>
       <c r="G2" t="n">
-        <v>1.02</v>
+        <v>1.019</v>
       </c>
       <c r="H2" t="n">
         <v>-73.09</v>
@@ -561,16 +561,16 @@
         <v>-17.88</v>
       </c>
       <c r="J2" t="n">
-        <v>29.71</v>
+        <v>29.705</v>
       </c>
       <c r="K2" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L2" t="n">
         <v>3.04</v>
       </c>
       <c r="M2" t="n">
-        <v>0.63</v>
+        <v>0.628</v>
       </c>
       <c r="N2" t="n">
         <v>-23.74</v>
@@ -579,16 +579,16 @@
         <v>5.94</v>
       </c>
       <c r="P2" t="n">
-        <v>118.42</v>
+        <v>118.423</v>
       </c>
       <c r="Q2" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R2" t="n">
-        <v>5.05</v>
+        <v>5.051</v>
       </c>
       <c r="S2" t="n">
-        <v>0.5</v>
+        <v>0.504</v>
       </c>
     </row>
     <row r="3">
@@ -604,16 +604,16 @@
         <v>17.88</v>
       </c>
       <c r="D3" t="n">
-        <v>29.71</v>
+        <v>29.705</v>
       </c>
       <c r="E3" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F3" t="n">
-        <v>5.05</v>
+        <v>5.051</v>
       </c>
       <c r="G3" t="n">
-        <v>1.02</v>
+        <v>1.019</v>
       </c>
       <c r="H3" t="n">
         <v>-73.09</v>
@@ -622,16 +622,16 @@
         <v>-17.88</v>
       </c>
       <c r="J3" t="n">
-        <v>29.71</v>
+        <v>29.705</v>
       </c>
       <c r="K3" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L3" t="n">
         <v>3.04</v>
       </c>
       <c r="M3" t="n">
-        <v>0.63</v>
+        <v>0.628</v>
       </c>
       <c r="N3" t="n">
         <v>-23.74</v>
@@ -640,16 +640,16 @@
         <v>5.94</v>
       </c>
       <c r="P3" t="n">
-        <v>118.42</v>
+        <v>118.423</v>
       </c>
       <c r="Q3" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R3" t="n">
-        <v>5.05</v>
+        <v>5.051</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0.504</v>
       </c>
     </row>
     <row r="4">
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-93.23</v>
+        <v>-93.235</v>
       </c>
       <c r="C4" t="n">
         <v>17.88</v>
@@ -668,10 +668,10 @@
         <v>29.61</v>
       </c>
       <c r="E4" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F4" t="n">
-        <v>4.83</v>
+        <v>4.831</v>
       </c>
       <c r="G4" t="n">
         <v>0.77</v>
@@ -686,31 +686,31 @@
         <v>29.61</v>
       </c>
       <c r="K4" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L4" t="n">
-        <v>3.23</v>
+        <v>3.228</v>
       </c>
       <c r="M4" t="n">
-        <v>0.53</v>
+        <v>0.533</v>
       </c>
       <c r="N4" t="n">
-        <v>-30.97</v>
+        <v>-30.974</v>
       </c>
       <c r="O4" t="n">
         <v>5.94</v>
       </c>
       <c r="P4" t="n">
-        <v>118.04</v>
+        <v>118.044</v>
       </c>
       <c r="Q4" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R4" t="n">
-        <v>4.83</v>
+        <v>4.831</v>
       </c>
       <c r="S4" t="n">
-        <v>0.48</v>
+        <v>0.481</v>
       </c>
     </row>
     <row r="5">
@@ -720,58 +720,58 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-93.37</v>
+        <v>-93.371</v>
       </c>
       <c r="C5" t="n">
         <v>17.88</v>
       </c>
       <c r="D5" t="n">
-        <v>29.61</v>
+        <v>29.612</v>
       </c>
       <c r="E5" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F5" t="n">
         <v>4.83</v>
       </c>
       <c r="G5" t="n">
-        <v>0.77</v>
+        <v>0.769</v>
       </c>
       <c r="H5" t="n">
-        <v>-93.90000000000001</v>
+        <v>-93.89700000000001</v>
       </c>
       <c r="I5" t="n">
         <v>-17.88</v>
       </c>
       <c r="J5" t="n">
-        <v>29.61</v>
+        <v>29.612</v>
       </c>
       <c r="K5" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L5" t="n">
-        <v>3.24</v>
+        <v>3.239</v>
       </c>
       <c r="M5" t="n">
-        <v>0.53</v>
+        <v>0.527</v>
       </c>
       <c r="N5" t="n">
-        <v>-31.02</v>
+        <v>-31.019</v>
       </c>
       <c r="O5" t="n">
         <v>5.94</v>
       </c>
       <c r="P5" t="n">
-        <v>118.05</v>
+        <v>118.049</v>
       </c>
       <c r="Q5" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R5" t="n">
         <v>4.83</v>
       </c>
       <c r="S5" t="n">
-        <v>0.48</v>
+        <v>0.481</v>
       </c>
     </row>
     <row r="6">
@@ -781,55 +781,55 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-92.72</v>
+        <v>-92.718</v>
       </c>
       <c r="C6" t="n">
         <v>17.88</v>
       </c>
       <c r="D6" t="n">
-        <v>30.06</v>
+        <v>30.064</v>
       </c>
       <c r="E6" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F6" t="n">
-        <v>4.84</v>
+        <v>4.836</v>
       </c>
       <c r="G6" t="n">
-        <v>0.77</v>
+        <v>0.773</v>
       </c>
       <c r="H6" t="n">
-        <v>-93.70999999999999</v>
+        <v>-93.708</v>
       </c>
       <c r="I6" t="n">
         <v>-17.88</v>
       </c>
       <c r="J6" t="n">
-        <v>30.06</v>
+        <v>30.064</v>
       </c>
       <c r="K6" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L6" t="n">
-        <v>3.24</v>
+        <v>3.237</v>
       </c>
       <c r="M6" t="n">
-        <v>0.53</v>
+        <v>0.527</v>
       </c>
       <c r="N6" t="n">
-        <v>-30.8</v>
+        <v>-30.802</v>
       </c>
       <c r="O6" t="n">
         <v>5.94</v>
       </c>
       <c r="P6" t="n">
-        <v>119.85</v>
+        <v>119.854</v>
       </c>
       <c r="Q6" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R6" t="n">
-        <v>4.84</v>
+        <v>4.836</v>
       </c>
       <c r="S6" t="n">
         <v>0.47</v>
@@ -842,58 +842,58 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-92.22</v>
+        <v>-92.224</v>
       </c>
       <c r="C7" t="n">
         <v>17.88</v>
       </c>
       <c r="D7" t="n">
-        <v>52.55</v>
+        <v>52.547</v>
       </c>
       <c r="E7" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F7" t="n">
-        <v>4.84</v>
+        <v>4.842</v>
       </c>
       <c r="G7" t="n">
-        <v>0.66</v>
+        <v>0.662</v>
       </c>
       <c r="H7" t="n">
-        <v>-93.26000000000001</v>
+        <v>-93.258</v>
       </c>
       <c r="I7" t="n">
         <v>-17.88</v>
       </c>
       <c r="J7" t="n">
-        <v>52.55</v>
+        <v>52.547</v>
       </c>
       <c r="K7" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L7" t="n">
-        <v>3.23</v>
+        <v>3.234</v>
       </c>
       <c r="M7" t="n">
-        <v>0.47</v>
+        <v>0.473</v>
       </c>
       <c r="N7" t="n">
-        <v>-30.64</v>
+        <v>-30.638</v>
       </c>
       <c r="O7" t="n">
         <v>5.94</v>
       </c>
       <c r="P7" t="n">
-        <v>209.48</v>
+        <v>209.481</v>
       </c>
       <c r="Q7" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R7" t="n">
-        <v>4.84</v>
+        <v>4.842</v>
       </c>
       <c r="S7" t="n">
-        <v>0.18</v>
+        <v>0.176</v>
       </c>
     </row>
     <row r="8">
@@ -903,58 +903,58 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-92.22</v>
+        <v>-92.224</v>
       </c>
       <c r="C8" t="n">
         <v>17.88</v>
       </c>
       <c r="D8" t="n">
-        <v>52.55</v>
+        <v>52.547</v>
       </c>
       <c r="E8" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F8" t="n">
-        <v>4.84</v>
+        <v>4.842</v>
       </c>
       <c r="G8" t="n">
-        <v>0.66</v>
+        <v>0.662</v>
       </c>
       <c r="H8" t="n">
-        <v>-93.26000000000001</v>
+        <v>-93.258</v>
       </c>
       <c r="I8" t="n">
         <v>-17.88</v>
       </c>
       <c r="J8" t="n">
-        <v>52.55</v>
+        <v>52.547</v>
       </c>
       <c r="K8" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L8" t="n">
-        <v>3.23</v>
+        <v>3.234</v>
       </c>
       <c r="M8" t="n">
-        <v>0.47</v>
+        <v>0.473</v>
       </c>
       <c r="N8" t="n">
-        <v>-30.64</v>
+        <v>-30.638</v>
       </c>
       <c r="O8" t="n">
         <v>5.94</v>
       </c>
       <c r="P8" t="n">
-        <v>209.48</v>
+        <v>209.481</v>
       </c>
       <c r="Q8" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R8" t="n">
-        <v>4.84</v>
+        <v>4.842</v>
       </c>
       <c r="S8" t="n">
-        <v>0.18</v>
+        <v>0.176</v>
       </c>
     </row>
     <row r="9">
@@ -964,55 +964,55 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-92.72</v>
+        <v>-92.718</v>
       </c>
       <c r="C9" t="n">
         <v>17.88</v>
       </c>
       <c r="D9" t="n">
-        <v>30.06</v>
+        <v>30.064</v>
       </c>
       <c r="E9" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F9" t="n">
-        <v>4.84</v>
+        <v>4.836</v>
       </c>
       <c r="G9" t="n">
-        <v>0.77</v>
+        <v>0.773</v>
       </c>
       <c r="H9" t="n">
-        <v>-93.70999999999999</v>
+        <v>-93.708</v>
       </c>
       <c r="I9" t="n">
         <v>-17.88</v>
       </c>
       <c r="J9" t="n">
-        <v>30.06</v>
+        <v>30.064</v>
       </c>
       <c r="K9" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L9" t="n">
-        <v>3.24</v>
+        <v>3.237</v>
       </c>
       <c r="M9" t="n">
-        <v>0.53</v>
+        <v>0.527</v>
       </c>
       <c r="N9" t="n">
-        <v>-30.8</v>
+        <v>-30.802</v>
       </c>
       <c r="O9" t="n">
         <v>5.94</v>
       </c>
       <c r="P9" t="n">
-        <v>119.85</v>
+        <v>119.854</v>
       </c>
       <c r="Q9" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R9" t="n">
-        <v>4.84</v>
+        <v>4.836</v>
       </c>
       <c r="S9" t="n">
         <v>0.47</v>
@@ -1025,58 +1025,58 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-93.37</v>
+        <v>-93.371</v>
       </c>
       <c r="C10" t="n">
         <v>17.88</v>
       </c>
       <c r="D10" t="n">
-        <v>29.61</v>
+        <v>29.612</v>
       </c>
       <c r="E10" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F10" t="n">
         <v>4.83</v>
       </c>
       <c r="G10" t="n">
-        <v>0.77</v>
+        <v>0.769</v>
       </c>
       <c r="H10" t="n">
-        <v>-93.90000000000001</v>
+        <v>-93.89700000000001</v>
       </c>
       <c r="I10" t="n">
         <v>-17.88</v>
       </c>
       <c r="J10" t="n">
-        <v>29.61</v>
+        <v>29.612</v>
       </c>
       <c r="K10" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L10" t="n">
-        <v>3.24</v>
+        <v>3.239</v>
       </c>
       <c r="M10" t="n">
-        <v>0.53</v>
+        <v>0.527</v>
       </c>
       <c r="N10" t="n">
-        <v>-31.02</v>
+        <v>-31.019</v>
       </c>
       <c r="O10" t="n">
         <v>5.94</v>
       </c>
       <c r="P10" t="n">
-        <v>118.05</v>
+        <v>118.049</v>
       </c>
       <c r="Q10" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R10" t="n">
         <v>4.83</v>
       </c>
       <c r="S10" t="n">
-        <v>0.48</v>
+        <v>0.481</v>
       </c>
     </row>
     <row r="11">
@@ -1086,7 +1086,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-93.23</v>
+        <v>-93.235</v>
       </c>
       <c r="C11" t="n">
         <v>17.88</v>
@@ -1095,10 +1095,10 @@
         <v>29.61</v>
       </c>
       <c r="E11" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F11" t="n">
-        <v>4.83</v>
+        <v>4.831</v>
       </c>
       <c r="G11" t="n">
         <v>0.77</v>
@@ -1113,31 +1113,31 @@
         <v>29.61</v>
       </c>
       <c r="K11" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L11" t="n">
-        <v>3.23</v>
+        <v>3.228</v>
       </c>
       <c r="M11" t="n">
-        <v>0.53</v>
+        <v>0.533</v>
       </c>
       <c r="N11" t="n">
-        <v>-30.97</v>
+        <v>-30.974</v>
       </c>
       <c r="O11" t="n">
         <v>5.94</v>
       </c>
       <c r="P11" t="n">
-        <v>118.04</v>
+        <v>118.044</v>
       </c>
       <c r="Q11" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R11" t="n">
-        <v>4.83</v>
+        <v>4.831</v>
       </c>
       <c r="S11" t="n">
-        <v>0.48</v>
+        <v>0.481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>